<commit_message>
Fix GitHub upload API parameter and add environment variable logging
</commit_message>
<xml_diff>
--- a/uploads/급여_리스.xlsx
+++ b/uploads/급여_리스.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\HanMi\ERP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9D249F-BDFF-4176-9664-F55CA7554B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924337EA-82E8-4194-B312-5482BEFC4014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{33410158-1FCC-471B-96FE-A3658D8E7CFC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{33410158-1FCC-471B-96FE-A3658D8E7CFC}"/>
   </bookViews>
   <sheets>
     <sheet name="01월" sheetId="1" r:id="rId1"/>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852D1C01-E82A-4AB0-8EA9-B4D0C83AA06B}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -612,7 +612,7 @@
         <v>2800000</v>
       </c>
       <c r="I2">
-        <v>487720</v>
+        <v>477720</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1830,7 +1830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC525E7-C1FA-459D-B5D0-3649A3A73FD5}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2716,7 +2716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0330D018-0C0A-49F0-89B7-FF2665318EF9}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>